<commit_message>
Update Software developer key technologies for Vancouver.xlsx
</commit_message>
<xml_diff>
--- a/Software developer key technologies for Vancouver.xlsx
+++ b/Software developer key technologies for Vancouver.xlsx
@@ -11,9 +11,6 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$36:$D$67</definedName>
   </definedNames>
@@ -625,83 +622,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -731,16 +662,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -753,20 +726,44 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1564,12 +1561,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="88000768"/>
-        <c:axId val="89837568"/>
+        <c:axId val="61671680"/>
+        <c:axId val="61689856"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="88000768"/>
+        <c:axId val="61671680"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1578,7 +1575,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89837568"/>
+        <c:crossAx val="61689856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1586,7 +1583,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89837568"/>
+        <c:axId val="61689856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1597,7 +1594,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="88000768"/>
+        <c:crossAx val="61671680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1742,23 +1739,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Лист1"/>
-      <sheetName val="Лист2"/>
-      <sheetName val="Лист3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2050,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P50" sqref="P50"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,196 +2040,196 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="53"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="60"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="60" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="51"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:18" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="51"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="62"/>
+      <c r="F4" s="27"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13" t="s">
+      <c r="B5" s="42"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="51"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="27"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="51"/>
+      <c r="F6" s="27"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="6">
         <v>13023</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="16" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="6">
         <v>1544</v>
       </c>
-      <c r="F7" s="51"/>
+      <c r="F7" s="27"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="6">
         <v>9069</v>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="16" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="6">
         <v>1073</v>
       </c>
-      <c r="F8" s="51"/>
+      <c r="F8" s="27"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="6">
         <v>3097</v>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="16" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="6">
         <v>341</v>
       </c>
-      <c r="F9" s="51"/>
+      <c r="F9" s="27"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="6">
         <v>792</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="16" t="s">
+      <c r="C10" s="3"/>
+      <c r="D10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="6">
         <v>74</v>
       </c>
-      <c r="F10" s="51"/>
+      <c r="F10" s="27"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B11" s="6">
         <v>329</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="16" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="6">
         <v>34</v>
       </c>
-      <c r="F11" s="51"/>
+      <c r="F11" s="27"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="51"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="27"/>
     </row>
     <row r="13" spans="1:18" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="27"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="31" t="s">
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="51"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="27"/>
       <c r="G14" t="s">
         <v>11</v>
       </c>
@@ -2258,16 +2238,16 @@
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="23">
+      <c r="B15" s="40"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="36">
         <v>597</v>
       </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="51"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="27"/>
       <c r="G15" t="s">
         <v>43</v>
       </c>
@@ -2276,16 +2256,16 @@
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="23">
+      <c r="B16" s="40"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="36">
         <v>489</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="51"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="27"/>
       <c r="G16" t="s">
         <v>21</v>
       </c>
@@ -2294,16 +2274,16 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="23">
+      <c r="B17" s="40"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="36">
         <v>457</v>
       </c>
-      <c r="E17" s="25"/>
-      <c r="F17" s="51"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="27"/>
       <c r="G17" t="s">
         <v>13</v>
       </c>
@@ -2312,16 +2292,16 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="23">
+      <c r="B18" s="40"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="36">
         <v>379</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="51"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="27"/>
       <c r="G18" t="s">
         <v>44</v>
       </c>
@@ -2330,16 +2310,16 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="23">
+      <c r="B19" s="40"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="36">
         <v>360</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="51"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="27"/>
       <c r="G19" t="s">
         <v>45</v>
       </c>
@@ -2348,16 +2328,16 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="23">
+      <c r="B20" s="40"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="36">
         <v>305</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="51"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="27"/>
       <c r="G20" t="s">
         <v>52</v>
       </c>
@@ -2366,16 +2346,16 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="23">
+      <c r="B21" s="40"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="36">
         <v>256</v>
       </c>
-      <c r="E21" s="25"/>
-      <c r="F21" s="51"/>
+      <c r="E21" s="37"/>
+      <c r="F21" s="27"/>
       <c r="G21" t="s">
         <v>46</v>
       </c>
@@ -2384,16 +2364,16 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="23">
+      <c r="B22" s="40"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="36">
         <v>244</v>
       </c>
-      <c r="E22" s="25"/>
-      <c r="F22" s="51"/>
+      <c r="E22" s="37"/>
+      <c r="F22" s="27"/>
       <c r="G22" t="s">
         <v>38</v>
       </c>
@@ -2402,16 +2382,16 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="23">
+      <c r="B23" s="40"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="36">
         <v>218</v>
       </c>
-      <c r="E23" s="25"/>
-      <c r="F23" s="51"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="27"/>
       <c r="G23" t="s">
         <v>47</v>
       </c>
@@ -2420,16 +2400,16 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="23">
+      <c r="B24" s="40"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="36">
         <v>206</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="51"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="27"/>
       <c r="G24" t="s">
         <v>48</v>
       </c>
@@ -2438,16 +2418,16 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="23">
+      <c r="B25" s="40"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="36">
         <v>174</v>
       </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="51"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="27"/>
       <c r="G25" t="s">
         <v>34</v>
       </c>
@@ -2456,16 +2436,16 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="23">
+      <c r="B26" s="40"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="36">
         <v>173</v>
       </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="51"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="27"/>
       <c r="G26" t="s">
         <v>49</v>
       </c>
@@ -2474,16 +2454,16 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="23">
+      <c r="B27" s="40"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="36">
         <v>130</v>
       </c>
-      <c r="E27" s="25"/>
-      <c r="F27" s="51"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="27"/>
       <c r="G27" t="s">
         <v>31</v>
       </c>
@@ -2492,16 +2472,16 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="23">
+      <c r="B28" s="40"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="36">
         <v>124</v>
       </c>
-      <c r="E28" s="25"/>
-      <c r="F28" s="51"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="27"/>
       <c r="G28" t="s">
         <v>29</v>
       </c>
@@ -2510,16 +2490,16 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="25"/>
-      <c r="D29" s="23">
+      <c r="B29" s="40"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="36">
         <v>65</v>
       </c>
-      <c r="E29" s="25"/>
-      <c r="F29" s="51"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="27"/>
       <c r="G29" t="s">
         <v>50</v>
       </c>
@@ -2528,16 +2508,16 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="23">
+      <c r="B30" s="40"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="36">
         <v>49</v>
       </c>
-      <c r="E30" s="25"/>
-      <c r="F30" s="51"/>
+      <c r="E30" s="37"/>
+      <c r="F30" s="27"/>
       <c r="G30" t="s">
         <v>51</v>
       </c>
@@ -2546,492 +2526,492 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="23">
+      <c r="B31" s="40"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="36">
         <v>22</v>
       </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="51"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="27"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="51"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="27"/>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="51"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
+      <c r="D33" s="45"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="27"/>
     </row>
     <row r="34" spans="1:8" ht="183.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="55"/>
-      <c r="B34" s="56"/>
-      <c r="C34" s="56"/>
-      <c r="D34" s="56"/>
-      <c r="E34" s="57"/>
-      <c r="F34" s="51"/>
+      <c r="A34" s="47"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="27"/>
     </row>
     <row r="35" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="44"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="42" t="s">
+      <c r="B35" s="22"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="43"/>
-      <c r="F35" s="51"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="27"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="33" t="s">
+      <c r="A36" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="35"/>
-      <c r="D36" s="45">
+      <c r="B36" s="12"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="23">
         <v>110</v>
       </c>
-      <c r="E36" s="35"/>
-      <c r="F36" s="51"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="27"/>
       <c r="H36" s="1"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
+      <c r="A37" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="37"/>
-      <c r="C37" s="38"/>
-      <c r="D37" s="46">
+      <c r="B37" s="15"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="24">
         <v>81</v>
       </c>
-      <c r="E37" s="38"/>
-      <c r="F37" s="51"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="27"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
+      <c r="A38" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="37"/>
-      <c r="C38" s="38"/>
-      <c r="D38" s="46">
+      <c r="B38" s="15"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="24">
         <v>48</v>
       </c>
-      <c r="E38" s="38"/>
-      <c r="F38" s="51"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="27"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="37"/>
-      <c r="C39" s="38"/>
-      <c r="D39" s="46">
+      <c r="B39" s="15"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="24">
         <v>45</v>
       </c>
-      <c r="E39" s="38"/>
-      <c r="F39" s="51"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="27"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="46">
+      <c r="B40" s="15"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="24">
         <v>41</v>
       </c>
-      <c r="E40" s="38"/>
-      <c r="F40" s="51"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="27"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="37"/>
-      <c r="C41" s="38"/>
-      <c r="D41" s="46">
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="24">
         <v>40</v>
       </c>
-      <c r="E41" s="38"/>
-      <c r="F41" s="51"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="27"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
+      <c r="A42" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="38"/>
-      <c r="D42" s="46">
+      <c r="B42" s="15"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="24">
         <v>37</v>
       </c>
-      <c r="E42" s="38"/>
-      <c r="F42" s="51"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="27"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B43" s="37"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="46">
+      <c r="B43" s="15"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="24">
         <v>34</v>
       </c>
-      <c r="E43" s="38"/>
-      <c r="F43" s="51"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="27"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
+      <c r="A44" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B44" s="37"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="46">
+      <c r="B44" s="15"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="24">
         <v>31</v>
       </c>
-      <c r="E44" s="38"/>
-      <c r="F44" s="51"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="27"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B45" s="37"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="46">
+      <c r="B45" s="15"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="24">
         <v>30</v>
       </c>
-      <c r="E45" s="38"/>
-      <c r="F45" s="51"/>
-      <c r="H45" s="22"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="27"/>
+      <c r="H45" s="10"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="36" t="s">
+      <c r="A46" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="37"/>
-      <c r="C46" s="38"/>
-      <c r="D46" s="46">
+      <c r="B46" s="15"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="24">
         <v>28</v>
       </c>
-      <c r="E46" s="38"/>
-      <c r="F46" s="51"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="27"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B47" s="37"/>
-      <c r="C47" s="38"/>
-      <c r="D47" s="46">
+      <c r="B47" s="15"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="24">
         <v>19</v>
       </c>
-      <c r="E47" s="38"/>
-      <c r="F47" s="51"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="27"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="39" t="s">
+      <c r="A48" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="37"/>
-      <c r="C48" s="38"/>
-      <c r="D48" s="46">
+      <c r="B48" s="15"/>
+      <c r="C48" s="16"/>
+      <c r="D48" s="24">
         <v>15</v>
       </c>
-      <c r="E48" s="38"/>
-      <c r="F48" s="51"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="27"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="36" t="s">
+      <c r="A49" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="37"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="46">
+      <c r="B49" s="15"/>
+      <c r="C49" s="16"/>
+      <c r="D49" s="24">
         <v>14</v>
       </c>
-      <c r="E49" s="38"/>
-      <c r="F49" s="51"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="27"/>
       <c r="H49" s="1"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="37"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="46">
+      <c r="B50" s="15"/>
+      <c r="C50" s="16"/>
+      <c r="D50" s="24">
         <v>13</v>
       </c>
-      <c r="E50" s="38"/>
-      <c r="F50" s="51"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="27"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="36" t="s">
+      <c r="A51" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B51" s="37"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="46">
+      <c r="B51" s="15"/>
+      <c r="C51" s="16"/>
+      <c r="D51" s="24">
         <v>12</v>
       </c>
-      <c r="E51" s="38"/>
-      <c r="F51" s="51"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="27"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="36" t="s">
+      <c r="A52" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B52" s="37"/>
-      <c r="C52" s="38"/>
-      <c r="D52" s="46">
+      <c r="B52" s="15"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="24">
         <v>10</v>
       </c>
-      <c r="E52" s="38"/>
-      <c r="F52" s="51"/>
-      <c r="H52" s="22"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="27"/>
+      <c r="H52" s="10"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="36" t="s">
+      <c r="A53" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B53" s="37"/>
-      <c r="C53" s="38"/>
-      <c r="D53" s="46">
+      <c r="B53" s="15"/>
+      <c r="C53" s="16"/>
+      <c r="D53" s="24">
         <v>6</v>
       </c>
-      <c r="E53" s="38"/>
-      <c r="F53" s="51"/>
-      <c r="H53" s="22"/>
+      <c r="E53" s="16"/>
+      <c r="F53" s="27"/>
+      <c r="H53" s="10"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="36" t="s">
+      <c r="A54" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B54" s="37"/>
-      <c r="C54" s="38"/>
-      <c r="D54" s="46">
+      <c r="B54" s="15"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="24">
         <v>5</v>
       </c>
-      <c r="E54" s="38"/>
-      <c r="F54" s="51"/>
-      <c r="H54" s="22"/>
+      <c r="E54" s="16"/>
+      <c r="F54" s="27"/>
+      <c r="H54" s="10"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="36" t="s">
+      <c r="A55" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B55" s="37"/>
-      <c r="C55" s="38"/>
-      <c r="D55" s="46">
+      <c r="B55" s="15"/>
+      <c r="C55" s="16"/>
+      <c r="D55" s="24">
         <v>5</v>
       </c>
-      <c r="E55" s="38"/>
-      <c r="F55" s="51"/>
-      <c r="H55" s="22"/>
+      <c r="E55" s="16"/>
+      <c r="F55" s="27"/>
+      <c r="H55" s="10"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="36" t="s">
+      <c r="A56" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B56" s="37"/>
-      <c r="C56" s="38"/>
-      <c r="D56" s="46">
+      <c r="B56" s="15"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="24">
         <v>4</v>
       </c>
-      <c r="E56" s="38"/>
-      <c r="F56" s="51"/>
-      <c r="H56" s="22"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="27"/>
+      <c r="H56" s="10"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="36" t="s">
+      <c r="A57" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B57" s="37"/>
-      <c r="C57" s="38"/>
-      <c r="D57" s="46">
+      <c r="B57" s="15"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="24">
         <v>4</v>
       </c>
-      <c r="E57" s="38"/>
-      <c r="F57" s="51"/>
-      <c r="H57" s="22"/>
+      <c r="E57" s="16"/>
+      <c r="F57" s="27"/>
+      <c r="H57" s="10"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="36" t="s">
+      <c r="A58" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B58" s="37"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="46">
+      <c r="B58" s="15"/>
+      <c r="C58" s="16"/>
+      <c r="D58" s="24">
         <v>2</v>
       </c>
-      <c r="E58" s="38"/>
-      <c r="F58" s="51"/>
-      <c r="H58" s="22"/>
+      <c r="E58" s="16"/>
+      <c r="F58" s="27"/>
+      <c r="H58" s="10"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="36" t="s">
+      <c r="A59" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="37"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="46">
+      <c r="B59" s="15"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="24">
         <v>2</v>
       </c>
-      <c r="E59" s="38"/>
-      <c r="F59" s="51"/>
-      <c r="H59" s="22"/>
+      <c r="E59" s="16"/>
+      <c r="F59" s="27"/>
+      <c r="H59" s="10"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="36" t="s">
+      <c r="A60" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B60" s="37"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="46">
+      <c r="B60" s="15"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="24">
         <v>2</v>
       </c>
-      <c r="E60" s="38"/>
-      <c r="F60" s="51"/>
-      <c r="H60" s="22"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="27"/>
+      <c r="H60" s="10"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="37" t="s">
+      <c r="A61" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B61" s="37"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="46">
+      <c r="B61" s="15"/>
+      <c r="C61" s="16"/>
+      <c r="D61" s="24">
         <v>2</v>
       </c>
-      <c r="E61" s="38"/>
-      <c r="F61" s="51"/>
-      <c r="H61" s="22"/>
+      <c r="E61" s="16"/>
+      <c r="F61" s="27"/>
+      <c r="H61" s="10"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="37" t="s">
+      <c r="A62" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="B62" s="37"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="46">
+      <c r="B62" s="15"/>
+      <c r="C62" s="16"/>
+      <c r="D62" s="24">
         <v>2</v>
       </c>
-      <c r="E62" s="38"/>
-      <c r="F62" s="51"/>
-      <c r="H62" s="22"/>
+      <c r="E62" s="16"/>
+      <c r="F62" s="27"/>
+      <c r="H62" s="10"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="37" t="s">
+      <c r="A63" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B63" s="37"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="46">
+      <c r="B63" s="15"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="24">
         <v>1</v>
       </c>
-      <c r="E63" s="38"/>
-      <c r="F63" s="51"/>
-      <c r="H63" s="22"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="27"/>
+      <c r="H63" s="10"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="37" t="s">
+      <c r="A64" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B64" s="37"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="46">
+      <c r="B64" s="15"/>
+      <c r="C64" s="16"/>
+      <c r="D64" s="24">
         <v>1</v>
       </c>
-      <c r="E64" s="38"/>
-      <c r="F64" s="51"/>
-      <c r="H64" s="22"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="27"/>
+      <c r="H64" s="10"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="37" t="s">
+      <c r="A65" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B65" s="37"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="46">
+      <c r="B65" s="15"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="24">
         <v>1</v>
       </c>
-      <c r="E65" s="38"/>
-      <c r="F65" s="51"/>
-      <c r="H65" s="22"/>
+      <c r="E65" s="16"/>
+      <c r="F65" s="27"/>
+      <c r="H65" s="10"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="37" t="s">
+      <c r="A66" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B66" s="37"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="46">
+      <c r="B66" s="15"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="24">
         <v>1</v>
       </c>
-      <c r="E66" s="38"/>
-      <c r="F66" s="51"/>
-      <c r="H66" s="22"/>
+      <c r="E66" s="16"/>
+      <c r="F66" s="27"/>
+      <c r="H66" s="10"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="40" t="s">
+      <c r="A67" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B67" s="40"/>
-      <c r="C67" s="41"/>
-      <c r="D67" s="47">
+      <c r="B67" s="18"/>
+      <c r="C67" s="19"/>
+      <c r="D67" s="25">
         <v>1</v>
       </c>
-      <c r="E67" s="41"/>
-      <c r="F67" s="51"/>
-      <c r="H67" s="22"/>
-    </row>
-    <row r="68" spans="1:8" ht="87" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="58" t="s">
+      <c r="E67" s="19"/>
+      <c r="F67" s="27"/>
+      <c r="H67" s="10"/>
+    </row>
+    <row r="68" spans="1:8" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B68" s="48"/>
-      <c r="C68" s="48"/>
-      <c r="D68" s="48"/>
-      <c r="E68" s="59"/>
-      <c r="F68" s="51"/>
-      <c r="H68" s="22"/>
+      <c r="B68" s="31"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="31"/>
+      <c r="E68" s="32"/>
+      <c r="F68" s="27"/>
+      <c r="H68" s="10"/>
     </row>
     <row r="69" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="60" t="s">
+      <c r="A69" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="B69" s="61"/>
-      <c r="C69" s="61"/>
-      <c r="D69" s="61"/>
-      <c r="E69" s="62"/>
-      <c r="F69" s="51"/>
+      <c r="B69" s="34"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="35"/>
+      <c r="F69" s="27"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="50"/>
-      <c r="B70" s="50"/>
-      <c r="C70" s="50"/>
-      <c r="D70" s="50"/>
-      <c r="E70" s="50"/>
-      <c r="F70" s="52"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="26"/>
+      <c r="D70" s="26"/>
+      <c r="E70" s="26"/>
+      <c r="F70" s="28"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="22"/>
+      <c r="A74" s="10"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="22"/>
+      <c r="A75" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="A36:D67">
@@ -3040,37 +3020,11 @@
     </sortState>
   </autoFilter>
   <mergeCells count="47">
-    <mergeCell ref="A68:E68"/>
-    <mergeCell ref="A69:E69"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A4:E4"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="D5:E5"/>
@@ -3082,11 +3036,37 @@
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A18:C18"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A1:R1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="A68:E68"/>
+    <mergeCell ref="A69:E69"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>